<commit_message>
changed hyperparameter to author recommendation, and completed readme on usage
</commit_message>
<xml_diff>
--- a/rankings-to-date.xlsx
+++ b/rankings-to-date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/19-20/varsity swimmin/isb-varsity-swimming-rankings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E801C556-7AFC-CD49-9103-8AD0D4F9271C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2943F49-06E4-6644-A55E-42FB146D557A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{13077E5F-9E70-7144-8AEE-7A649CDE6306}"/>
   </bookViews>
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6A47F1-213F-184D-8EE4-A22310B61320}">
   <dimension ref="A1:F290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <f t="shared" ref="A258:A321" si="4">SUMPRODUCT((D258=D$3:D$291)*(E258=E$3:E$291)*(B258&gt;B$3:B$291))+1</f>
+        <f t="shared" ref="A258:A290" si="4">SUMPRODUCT((D258=D$3:D$291)*(E258=E$3:E$291)*(B258&gt;B$3:B$291))+1</f>
         <v>9</v>
       </c>
       <c r="B258" s="2" t="s">

</xml_diff>

<commit_message>
added design document which inlucdes MVP
</commit_message>
<xml_diff>
--- a/rankings-to-date.xlsx
+++ b/rankings-to-date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alansun/Documents/19-20/varsity swimmin/isb-varsity-swimming-rankings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2943F49-06E4-6644-A55E-42FB146D557A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842F8A35-35AC-3448-8C84-20F81932393B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{13077E5F-9E70-7144-8AEE-7A649CDE6306}"/>
   </bookViews>
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6A47F1-213F-184D-8EE4-A22310B61320}">
   <dimension ref="A1:F290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>